<commit_message>
backend: Excel import -> improved email validation
</commit_message>
<xml_diff>
--- a/users_app/test_data/import_template_multi_column_sort_EXAMPLE.xlsx
+++ b/users_app/test_data/import_template_multi_column_sort_EXAMPLE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -35,6 +35,114 @@
   </si>
   <si>
     <t xml:space="preserve">bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.multi.column.sort@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_test</t>
   </si>
 </sst>
 </file>
@@ -402,12 +510,12 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E135" activeCellId="0" sqref="A2:E135"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.91"/>
@@ -431,32 +539,277 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="3"/>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="3"/>

</xml_diff>